<commit_message>
Added dmamux resources for STM32G431.
</commit_message>
<xml_diff>
--- a/altfun/stm32g431.xlsx
+++ b/altfun/stm32g431.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\hal\altfun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB60657-C3E6-40BF-AEA2-6002D012611C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB0BDAC-FC2B-4C06-B0C9-2F52E677919A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="180" windowWidth="35820" windowHeight="20775" xr2:uid="{13F91BF3-55E2-4A0E-B090-1607FC0C82C4}"/>
+    <workbookView xWindow="21990" yWindow="7065" windowWidth="25995" windowHeight="27900" activeTab="2" xr2:uid="{13F91BF3-55E2-4A0E-B090-1607FC0C82C4}"/>
   </bookViews>
   <sheets>
     <sheet name="pinout" sheetId="1" r:id="rId1"/>
     <sheet name="altfun" sheetId="2" r:id="rId2"/>
+    <sheet name="dmamux" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_bookmark0" localSheetId="1">altfun!#REF!</definedName>
@@ -325,7 +326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2621" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2742" uniqueCount="597">
   <si>
     <t>Alternate function</t>
   </si>
@@ -1887,6 +1888,258 @@
   </si>
   <si>
     <t>SPI3_MOSI,I2S3_SD</t>
+  </si>
+  <si>
+    <t>TIM20_CH2</t>
+  </si>
+  <si>
+    <t>TIM20_CH3</t>
+  </si>
+  <si>
+    <t>TIM1_UP</t>
+  </si>
+  <si>
+    <t>TIM20_CH4</t>
+  </si>
+  <si>
+    <t>TIM1_TRIG</t>
+  </si>
+  <si>
+    <t>TIM20_UP</t>
+  </si>
+  <si>
+    <t>ADC1</t>
+  </si>
+  <si>
+    <t>TIM1_COM</t>
+  </si>
+  <si>
+    <t>AES_IN</t>
+  </si>
+  <si>
+    <t>DAC1_CH1</t>
+  </si>
+  <si>
+    <t>AES_OUT</t>
+  </si>
+  <si>
+    <t>DAC1_CH2</t>
+  </si>
+  <si>
+    <t>TIM20_TRIG</t>
+  </si>
+  <si>
+    <t>TIM6_UP</t>
+  </si>
+  <si>
+    <t>TIM20_COM</t>
+  </si>
+  <si>
+    <t>TIM7_UP</t>
+  </si>
+  <si>
+    <t>HRTIM_MASTER</t>
+  </si>
+  <si>
+    <t>SPI1_RX</t>
+  </si>
+  <si>
+    <t>TIM8_UP</t>
+  </si>
+  <si>
+    <t>HRTIM_TIMA</t>
+  </si>
+  <si>
+    <t>SPI1_TX</t>
+  </si>
+  <si>
+    <t>TIM8_TRIG</t>
+  </si>
+  <si>
+    <t>HRTIM_TIMB</t>
+  </si>
+  <si>
+    <t>SPI2_RX</t>
+  </si>
+  <si>
+    <t>TIM8_COM</t>
+  </si>
+  <si>
+    <t>HRTIM_TIMC</t>
+  </si>
+  <si>
+    <t>SPI2_TX</t>
+  </si>
+  <si>
+    <t>HRTIM_TIMD</t>
+  </si>
+  <si>
+    <t>SPI3_RX</t>
+  </si>
+  <si>
+    <t>HRTIM_TIME</t>
+  </si>
+  <si>
+    <t>SPI3_TX</t>
+  </si>
+  <si>
+    <t>HRTIM_TIMF</t>
+  </si>
+  <si>
+    <t>I2C1_RX</t>
+  </si>
+  <si>
+    <t>DAC3_CH1</t>
+  </si>
+  <si>
+    <t>I2C1_TX</t>
+  </si>
+  <si>
+    <t>TIM2_UP</t>
+  </si>
+  <si>
+    <t>DAC3_CH2</t>
+  </si>
+  <si>
+    <t>I2C2_RX</t>
+  </si>
+  <si>
+    <t>DAC4_CH1</t>
+  </si>
+  <si>
+    <t>I2C2_TX</t>
+  </si>
+  <si>
+    <t>DAC4_CH2</t>
+  </si>
+  <si>
+    <t>I2C3_RX</t>
+  </si>
+  <si>
+    <t>SPI4_RX</t>
+  </si>
+  <si>
+    <t>I2C3_TX</t>
+  </si>
+  <si>
+    <t>SPI4_TX</t>
+  </si>
+  <si>
+    <t>I2C4_RX</t>
+  </si>
+  <si>
+    <t>TIM3_UP</t>
+  </si>
+  <si>
+    <t>SAI1_A</t>
+  </si>
+  <si>
+    <t>I2C4_TX</t>
+  </si>
+  <si>
+    <t>TIM3_TRIG</t>
+  </si>
+  <si>
+    <t>SAI1_B</t>
+  </si>
+  <si>
+    <t>FMAC_Read</t>
+  </si>
+  <si>
+    <t>FMAC_Write</t>
+  </si>
+  <si>
+    <t>Cordic_Read</t>
+  </si>
+  <si>
+    <t>Cordic_Write</t>
+  </si>
+  <si>
+    <t>TIM4_UP</t>
+  </si>
+  <si>
+    <t>UCPD1_RX</t>
+  </si>
+  <si>
+    <t>TIM5_CH1</t>
+  </si>
+  <si>
+    <t>UCPD1_TX</t>
+  </si>
+  <si>
+    <t>TIM5_CH2</t>
+  </si>
+  <si>
+    <t>TIM5_CH3</t>
+  </si>
+  <si>
+    <t>UART5_RX</t>
+  </si>
+  <si>
+    <t>TIM5_CH4</t>
+  </si>
+  <si>
+    <t>UART5_TX</t>
+  </si>
+  <si>
+    <t>TIM5_UP</t>
+  </si>
+  <si>
+    <t>TIM5_TRIG</t>
+  </si>
+  <si>
+    <t>ADC2</t>
+  </si>
+  <si>
+    <t>TIM15_UP</t>
+  </si>
+  <si>
+    <t>ADC3</t>
+  </si>
+  <si>
+    <t>TIM15_TRIG</t>
+  </si>
+  <si>
+    <t>ADC4</t>
+  </si>
+  <si>
+    <t>TIM15_COM</t>
+  </si>
+  <si>
+    <t>ADC5</t>
+  </si>
+  <si>
+    <t>QUADSPI</t>
+  </si>
+  <si>
+    <t>TIM16_UP</t>
+  </si>
+  <si>
+    <t>DAC2_CH1</t>
+  </si>
+  <si>
+    <t>TIM17_UP</t>
+  </si>
+  <si>
+    <t>TIM20_CH1</t>
+  </si>
+  <si>
+    <t>DMAMUX_Req_G0</t>
+  </si>
+  <si>
+    <t>DMAMUX_Req_G1</t>
+  </si>
+  <si>
+    <t>DMAMUX_ReqG2</t>
+  </si>
+  <si>
+    <t>DMAMUX_Req_G3</t>
+  </si>
+  <si>
+    <t>resource</t>
+  </si>
+  <si>
+    <t>mux input</t>
   </si>
 </sst>
 </file>
@@ -2139,7 +2392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2219,6 +2472,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2231,9 +2487,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2930,8 +3184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18723A7F-6928-421B-BC06-1255A474CE1C}">
   <dimension ref="B3:P126"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView showGridLines="0" topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8091,7 +8345,7 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="30" t="s">
         <v>339</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -8147,7 +8401,7 @@
       </c>
     </row>
     <row r="11" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="30"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="5" t="s">
         <v>50</v>
       </c>
@@ -8201,7 +8455,7 @@
       </c>
     </row>
     <row r="12" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="30"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="5" t="s">
         <v>54</v>
       </c>
@@ -8255,7 +8509,7 @@
       </c>
     </row>
     <row r="13" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="30"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="5" t="s">
         <v>63</v>
       </c>
@@ -8309,7 +8563,7 @@
       </c>
     </row>
     <row r="14" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="30"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="5" t="s">
         <v>46</v>
       </c>
@@ -8363,7 +8617,7 @@
       </c>
     </row>
     <row r="15" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="30"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="5" t="s">
         <v>51</v>
       </c>
@@ -8417,7 +8671,7 @@
       </c>
     </row>
     <row r="16" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="30"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="5" t="s">
         <v>59</v>
       </c>
@@ -8471,7 +8725,7 @@
       </c>
     </row>
     <row r="17" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="30"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="5" t="s">
         <v>64</v>
       </c>
@@ -8525,7 +8779,7 @@
       </c>
     </row>
     <row r="18" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="30"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
@@ -8579,7 +8833,7 @@
       </c>
     </row>
     <row r="19" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="30"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="5" t="s">
         <v>5</v>
       </c>
@@ -8633,7 +8887,7 @@
       </c>
     </row>
     <row r="20" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="30"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="5" t="s">
         <v>4</v>
       </c>
@@ -8687,7 +8941,7 @@
       </c>
     </row>
     <row r="21" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="30"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="5" t="s">
         <v>11</v>
       </c>
@@ -8741,7 +8995,7 @@
       </c>
     </row>
     <row r="22" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="30"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="5" t="s">
         <v>10</v>
       </c>
@@ -8795,7 +9049,7 @@
       </c>
     </row>
     <row r="23" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="30"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="5" t="s">
         <v>9</v>
       </c>
@@ -8849,7 +9103,7 @@
       </c>
     </row>
     <row r="24" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="30"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="5" t="s">
         <v>8</v>
       </c>
@@ -8903,7 +9157,7 @@
       </c>
     </row>
     <row r="25" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="31"/>
+      <c r="B25" s="32"/>
       <c r="C25" s="5" t="s">
         <v>32</v>
       </c>
@@ -8957,7 +9211,7 @@
       </c>
     </row>
     <row r="26" spans="2:19" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="30" t="s">
         <v>380</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -9013,7 +9267,7 @@
       </c>
     </row>
     <row r="27" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="30"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="5" t="s">
         <v>56</v>
       </c>
@@ -9067,7 +9321,7 @@
       </c>
     </row>
     <row r="28" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="30"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="5" t="s">
         <v>65</v>
       </c>
@@ -9121,7 +9375,7 @@
       </c>
     </row>
     <row r="29" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="30"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="5" t="s">
         <v>30</v>
       </c>
@@ -9175,7 +9429,7 @@
       </c>
     </row>
     <row r="30" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="30"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="5" t="s">
         <v>41</v>
       </c>
@@ -9229,7 +9483,7 @@
       </c>
     </row>
     <row r="31" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="30"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="5" t="s">
         <v>35</v>
       </c>
@@ -9283,7 +9537,7 @@
       </c>
     </row>
     <row r="32" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="30"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="5" t="s">
         <v>29</v>
       </c>
@@ -9337,7 +9591,7 @@
       </c>
     </row>
     <row r="33" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="30"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="5" t="s">
         <v>28</v>
       </c>
@@ -9391,7 +9645,7 @@
       </c>
     </row>
     <row r="34" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="30"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="5" t="s">
         <v>388</v>
       </c>
@@ -9445,7 +9699,7 @@
       </c>
     </row>
     <row r="35" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="30"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="5" t="s">
         <v>27</v>
       </c>
@@ -9499,7 +9753,7 @@
       </c>
     </row>
     <row r="36" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="30"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="5" t="s">
         <v>67</v>
       </c>
@@ -9553,7 +9807,7 @@
       </c>
     </row>
     <row r="37" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="30"/>
+      <c r="B37" s="31"/>
       <c r="C37" s="5" t="s">
         <v>17</v>
       </c>
@@ -9607,7 +9861,7 @@
       </c>
     </row>
     <row r="38" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="30"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="5" t="s">
         <v>16</v>
       </c>
@@ -9661,7 +9915,7 @@
       </c>
     </row>
     <row r="39" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="30"/>
+      <c r="B39" s="31"/>
       <c r="C39" s="5" t="s">
         <v>15</v>
       </c>
@@ -9715,7 +9969,7 @@
       </c>
     </row>
     <row r="40" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="30"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="5" t="s">
         <v>14</v>
       </c>
@@ -9769,7 +10023,7 @@
       </c>
     </row>
     <row r="41" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="31"/>
+      <c r="B41" s="32"/>
       <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
@@ -9823,7 +10077,7 @@
       </c>
     </row>
     <row r="42" spans="2:19" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -9879,7 +10133,7 @@
       </c>
     </row>
     <row r="43" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="30"/>
+      <c r="B43" s="31"/>
       <c r="C43" s="5" t="s">
         <v>40</v>
       </c>
@@ -9933,7 +10187,7 @@
       </c>
     </row>
     <row r="44" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="30"/>
+      <c r="B44" s="31"/>
       <c r="C44" s="5" t="s">
         <v>45</v>
       </c>
@@ -9987,7 +10241,7 @@
       </c>
     </row>
     <row r="45" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="30"/>
+      <c r="B45" s="31"/>
       <c r="C45" s="5" t="s">
         <v>57</v>
       </c>
@@ -10041,7 +10295,7 @@
       </c>
     </row>
     <row r="46" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="30"/>
+      <c r="B46" s="31"/>
       <c r="C46" s="5" t="s">
         <v>47</v>
       </c>
@@ -10095,7 +10349,7 @@
       </c>
     </row>
     <row r="47" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="30"/>
+      <c r="B47" s="31"/>
       <c r="C47" s="5" t="s">
         <v>55</v>
       </c>
@@ -10149,7 +10403,7 @@
       </c>
     </row>
     <row r="48" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="30"/>
+      <c r="B48" s="31"/>
       <c r="C48" s="5" t="s">
         <v>23</v>
       </c>
@@ -10203,7 +10457,7 @@
       </c>
     </row>
     <row r="49" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="30"/>
+      <c r="B49" s="31"/>
       <c r="C49" s="5" t="s">
         <v>22</v>
       </c>
@@ -10257,7 +10511,7 @@
       </c>
     </row>
     <row r="50" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="30"/>
+      <c r="B50" s="31"/>
       <c r="C50" s="5" t="s">
         <v>21</v>
       </c>
@@ -10311,7 +10565,7 @@
       </c>
     </row>
     <row r="51" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="30"/>
+      <c r="B51" s="31"/>
       <c r="C51" s="5" t="s">
         <v>20</v>
       </c>
@@ -10365,7 +10619,7 @@
       </c>
     </row>
     <row r="52" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="30"/>
+      <c r="B52" s="31"/>
       <c r="C52" s="5" t="s">
         <v>42</v>
       </c>
@@ -10419,7 +10673,7 @@
       </c>
     </row>
     <row r="53" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="30"/>
+      <c r="B53" s="31"/>
       <c r="C53" s="5" t="s">
         <v>37</v>
       </c>
@@ -10473,7 +10727,7 @@
       </c>
     </row>
     <row r="54" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="30"/>
+      <c r="B54" s="31"/>
       <c r="C54" s="5" t="s">
         <v>31</v>
       </c>
@@ -10527,7 +10781,7 @@
       </c>
     </row>
     <row r="55" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="30"/>
+      <c r="B55" s="31"/>
       <c r="C55" s="5" t="s">
         <v>33</v>
       </c>
@@ -10581,7 +10835,7 @@
       </c>
     </row>
     <row r="56" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="30"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="5" t="s">
         <v>397</v>
       </c>
@@ -10635,7 +10889,7 @@
       </c>
     </row>
     <row r="57" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="31"/>
+      <c r="B57" s="32"/>
       <c r="C57" s="5" t="s">
         <v>398</v>
       </c>
@@ -10689,7 +10943,7 @@
       </c>
     </row>
     <row r="58" spans="2:19" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C58" s="5" t="s">
@@ -10745,7 +10999,7 @@
       </c>
     </row>
     <row r="59" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="30"/>
+      <c r="B59" s="31"/>
       <c r="C59" s="5" t="s">
         <v>269</v>
       </c>
@@ -10799,7 +11053,7 @@
       </c>
     </row>
     <row r="60" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="30"/>
+      <c r="B60" s="31"/>
       <c r="C60" s="5" t="s">
         <v>36</v>
       </c>
@@ -10853,7 +11107,7 @@
       </c>
     </row>
     <row r="61" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="30"/>
+      <c r="B61" s="31"/>
       <c r="C61" s="5" t="s">
         <v>273</v>
       </c>
@@ -10907,7 +11161,7 @@
       </c>
     </row>
     <row r="62" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="30"/>
+      <c r="B62" s="31"/>
       <c r="C62" s="5" t="s">
         <v>274</v>
       </c>
@@ -10961,7 +11215,7 @@
       </c>
     </row>
     <row r="63" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="30"/>
+      <c r="B63" s="31"/>
       <c r="C63" s="5" t="s">
         <v>276</v>
       </c>
@@ -11015,7 +11269,7 @@
       </c>
     </row>
     <row r="64" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="30"/>
+      <c r="B64" s="31"/>
       <c r="C64" s="5" t="s">
         <v>278</v>
       </c>
@@ -11069,7 +11323,7 @@
       </c>
     </row>
     <row r="65" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="30"/>
+      <c r="B65" s="31"/>
       <c r="C65" s="5" t="s">
         <v>279</v>
       </c>
@@ -11123,7 +11377,7 @@
       </c>
     </row>
     <row r="66" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="30"/>
+      <c r="B66" s="31"/>
       <c r="C66" s="5" t="s">
         <v>26</v>
       </c>
@@ -11177,7 +11431,7 @@
       </c>
     </row>
     <row r="67" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="30"/>
+      <c r="B67" s="31"/>
       <c r="C67" s="5" t="s">
         <v>25</v>
       </c>
@@ -11231,7 +11485,7 @@
       </c>
     </row>
     <row r="68" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="30"/>
+      <c r="B68" s="31"/>
       <c r="C68" s="5" t="s">
         <v>24</v>
       </c>
@@ -11285,7 +11539,7 @@
       </c>
     </row>
     <row r="69" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="30"/>
+      <c r="B69" s="31"/>
       <c r="C69" s="5" t="s">
         <v>72</v>
       </c>
@@ -11339,7 +11593,7 @@
       </c>
     </row>
     <row r="70" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="30"/>
+      <c r="B70" s="31"/>
       <c r="C70" s="5" t="s">
         <v>71</v>
       </c>
@@ -11393,7 +11647,7 @@
       </c>
     </row>
     <row r="71" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="30"/>
+      <c r="B71" s="31"/>
       <c r="C71" s="5" t="s">
         <v>70</v>
       </c>
@@ -11447,7 +11701,7 @@
       </c>
     </row>
     <row r="72" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="30"/>
+      <c r="B72" s="31"/>
       <c r="C72" s="5" t="s">
         <v>69</v>
       </c>
@@ -11501,7 +11755,7 @@
       </c>
     </row>
     <row r="73" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="31"/>
+      <c r="B73" s="32"/>
       <c r="C73" s="5" t="s">
         <v>68</v>
       </c>
@@ -11555,7 +11809,7 @@
       </c>
     </row>
     <row r="74" spans="2:19" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="29" t="s">
+      <c r="B74" s="30" t="s">
         <v>403</v>
       </c>
       <c r="C74" s="5" t="s">
@@ -11611,7 +11865,7 @@
       </c>
     </row>
     <row r="75" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="30"/>
+      <c r="B75" s="31"/>
       <c r="C75" s="5" t="s">
         <v>297</v>
       </c>
@@ -11665,7 +11919,7 @@
       </c>
     </row>
     <row r="76" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="30"/>
+      <c r="B76" s="31"/>
       <c r="C76" s="5" t="s">
         <v>90</v>
       </c>
@@ -11719,7 +11973,7 @@
       </c>
     </row>
     <row r="77" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="30"/>
+      <c r="B77" s="31"/>
       <c r="C77" s="5" t="s">
         <v>92</v>
       </c>
@@ -11773,7 +12027,7 @@
       </c>
     </row>
     <row r="78" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="30"/>
+      <c r="B78" s="31"/>
       <c r="C78" s="5" t="s">
         <v>94</v>
       </c>
@@ -11827,7 +12081,7 @@
       </c>
     </row>
     <row r="79" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="30"/>
+      <c r="B79" s="31"/>
       <c r="C79" s="5" t="s">
         <v>96</v>
       </c>
@@ -11881,7 +12135,7 @@
       </c>
     </row>
     <row r="80" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="30"/>
+      <c r="B80" s="31"/>
       <c r="C80" s="5" t="s">
         <v>98</v>
       </c>
@@ -11935,7 +12189,7 @@
       </c>
     </row>
     <row r="81" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="30"/>
+      <c r="B81" s="31"/>
       <c r="C81" s="5" t="s">
         <v>193</v>
       </c>
@@ -11989,7 +12243,7 @@
       </c>
     </row>
     <row r="82" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="30"/>
+      <c r="B82" s="31"/>
       <c r="C82" s="5" t="s">
         <v>196</v>
       </c>
@@ -12043,7 +12297,7 @@
       </c>
     </row>
     <row r="83" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="30"/>
+      <c r="B83" s="31"/>
       <c r="C83" s="5" t="s">
         <v>199</v>
       </c>
@@ -12097,7 +12351,7 @@
       </c>
     </row>
     <row r="84" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="30"/>
+      <c r="B84" s="31"/>
       <c r="C84" s="5" t="s">
         <v>201</v>
       </c>
@@ -12151,7 +12405,7 @@
       </c>
     </row>
     <row r="85" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="30"/>
+      <c r="B85" s="31"/>
       <c r="C85" s="5" t="s">
         <v>203</v>
       </c>
@@ -12205,7 +12459,7 @@
       </c>
     </row>
     <row r="86" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="30"/>
+      <c r="B86" s="31"/>
       <c r="C86" s="5" t="s">
         <v>205</v>
       </c>
@@ -12259,7 +12513,7 @@
       </c>
     </row>
     <row r="87" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="30"/>
+      <c r="B87" s="31"/>
       <c r="C87" s="5" t="s">
         <v>207</v>
       </c>
@@ -12313,7 +12567,7 @@
       </c>
     </row>
     <row r="88" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="30"/>
+      <c r="B88" s="31"/>
       <c r="C88" s="5" t="s">
         <v>209</v>
       </c>
@@ -12367,7 +12621,7 @@
       </c>
     </row>
     <row r="89" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="31"/>
+      <c r="B89" s="32"/>
       <c r="C89" s="5" t="s">
         <v>211</v>
       </c>
@@ -12421,7 +12675,7 @@
       </c>
     </row>
     <row r="90" spans="2:19" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="29" t="s">
+      <c r="B90" s="30" t="s">
         <v>409</v>
       </c>
       <c r="C90" s="5" t="s">
@@ -12477,7 +12731,7 @@
       </c>
     </row>
     <row r="91" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="30"/>
+      <c r="B91" s="31"/>
       <c r="C91" s="5" t="s">
         <v>411</v>
       </c>
@@ -12531,7 +12785,7 @@
       </c>
     </row>
     <row r="92" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="30"/>
+      <c r="B92" s="31"/>
       <c r="C92" s="5" t="s">
         <v>143</v>
       </c>
@@ -12585,7 +12839,7 @@
       </c>
     </row>
     <row r="93" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="30"/>
+      <c r="B93" s="31"/>
       <c r="C93" s="5" t="s">
         <v>113</v>
       </c>
@@ -12639,7 +12893,7 @@
       </c>
     </row>
     <row r="94" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="32"/>
+      <c r="B94" s="33"/>
       <c r="C94" s="5" t="s">
         <v>115</v>
       </c>
@@ -12693,7 +12947,7 @@
       </c>
     </row>
     <row r="95" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="33" t="s">
+      <c r="B95" s="29" t="s">
         <v>415</v>
       </c>
       <c r="C95" s="5" t="s">
@@ -12756,13 +13010,973 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B90:B94"/>
     <mergeCell ref="B10:B25"/>
     <mergeCell ref="B26:B41"/>
     <mergeCell ref="B42:B57"/>
     <mergeCell ref="B58:B73"/>
     <mergeCell ref="B74:B89"/>
-    <mergeCell ref="B90:B94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2CA4B0-0F72-4E85-9754-150406B1F781}">
+  <dimension ref="B3:F118"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="34" t="s">
+        <v>595</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>591</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>592</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>593</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>594</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>519</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>522</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>524</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>526</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>528</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>530</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>533</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>536</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>539</v>
+      </c>
+      <c r="C16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>541</v>
+      </c>
+      <c r="C17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>543</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>545</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>547</v>
+      </c>
+      <c r="C20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>550</v>
+      </c>
+      <c r="C21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>552</v>
+      </c>
+      <c r="C22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>554</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>556</v>
+      </c>
+      <c r="C24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>558</v>
+      </c>
+      <c r="C25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>561</v>
+      </c>
+      <c r="C26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>468</v>
+      </c>
+      <c r="C27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>463</v>
+      </c>
+      <c r="C28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>451</v>
+      </c>
+      <c r="C29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>447</v>
+      </c>
+      <c r="C30">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>499</v>
+      </c>
+      <c r="C31">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>500</v>
+      </c>
+      <c r="C32">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>396</v>
+      </c>
+      <c r="C33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>395</v>
+      </c>
+      <c r="C34">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>574</v>
+      </c>
+      <c r="C35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>576</v>
+      </c>
+      <c r="C36">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>452</v>
+      </c>
+      <c r="C37">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>449</v>
+      </c>
+      <c r="C38">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>579</v>
+      </c>
+      <c r="C39">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>581</v>
+      </c>
+      <c r="C40">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>583</v>
+      </c>
+      <c r="C41">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>585</v>
+      </c>
+      <c r="C42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>586</v>
+      </c>
+      <c r="C43">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>588</v>
+      </c>
+      <c r="C44">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>356</v>
+      </c>
+      <c r="C45">
+        <v>42</v>
+      </c>
+      <c r="E45" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>361</v>
+      </c>
+      <c r="C46">
+        <v>43</v>
+      </c>
+      <c r="E46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>365</v>
+      </c>
+      <c r="C47">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>369</v>
+      </c>
+      <c r="C48">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>515</v>
+      </c>
+      <c r="C49">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>517</v>
+      </c>
+      <c r="C50">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>520</v>
+      </c>
+      <c r="C51">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>379</v>
+      </c>
+      <c r="C52">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>377</v>
+      </c>
+      <c r="C53">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>391</v>
+      </c>
+      <c r="C54">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>400</v>
+      </c>
+      <c r="C55">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>531</v>
+      </c>
+      <c r="C56">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>534</v>
+      </c>
+      <c r="C57">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>537</v>
+      </c>
+      <c r="C58">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>442</v>
+      </c>
+      <c r="C59">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>401</v>
+      </c>
+      <c r="C60">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>362</v>
+      </c>
+      <c r="C61">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>366</v>
+      </c>
+      <c r="C62">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>548</v>
+      </c>
+      <c r="C63">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>348</v>
+      </c>
+      <c r="C64">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>344</v>
+      </c>
+      <c r="C65">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>381</v>
+      </c>
+      <c r="C66">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>382</v>
+      </c>
+      <c r="C67">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>559</v>
+      </c>
+      <c r="C68">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>562</v>
+      </c>
+      <c r="C69">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>368</v>
+      </c>
+      <c r="C70">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>371</v>
+      </c>
+      <c r="C71">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>375</v>
+      </c>
+      <c r="C72">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>389</v>
+      </c>
+      <c r="C73">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>568</v>
+      </c>
+      <c r="C74">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>570</v>
+      </c>
+      <c r="C75">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>572</v>
+      </c>
+      <c r="C76">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>573</v>
+      </c>
+      <c r="C77">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>575</v>
+      </c>
+      <c r="C78">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>577</v>
+      </c>
+      <c r="C79">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>578</v>
+      </c>
+      <c r="C80">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>412</v>
+      </c>
+      <c r="C81">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>580</v>
+      </c>
+      <c r="C82">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>582</v>
+      </c>
+      <c r="C83">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>584</v>
+      </c>
+      <c r="C84">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>455</v>
+      </c>
+      <c r="C85">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>587</v>
+      </c>
+      <c r="C86">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>457</v>
+      </c>
+      <c r="C87">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>589</v>
+      </c>
+      <c r="C88">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>590</v>
+      </c>
+      <c r="C89">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>513</v>
+      </c>
+      <c r="C90">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>514</v>
+      </c>
+      <c r="C91">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>516</v>
+      </c>
+      <c r="C92">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>518</v>
+      </c>
+      <c r="C93">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>521</v>
+      </c>
+      <c r="C94">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>523</v>
+      </c>
+      <c r="C95">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>525</v>
+      </c>
+      <c r="C96">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>527</v>
+      </c>
+      <c r="C97">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>529</v>
+      </c>
+      <c r="C98">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>532</v>
+      </c>
+      <c r="C99">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>535</v>
+      </c>
+      <c r="C100">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>538</v>
+      </c>
+      <c r="C101">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>540</v>
+      </c>
+      <c r="C102">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>542</v>
+      </c>
+      <c r="C103">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>544</v>
+      </c>
+      <c r="C104">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>546</v>
+      </c>
+      <c r="C105">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>549</v>
+      </c>
+      <c r="C106">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>551</v>
+      </c>
+      <c r="C107">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>553</v>
+      </c>
+      <c r="C108">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>555</v>
+      </c>
+      <c r="C109">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>557</v>
+      </c>
+      <c r="C110">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>560</v>
+      </c>
+      <c r="C111">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>563</v>
+      </c>
+      <c r="C112">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>564</v>
+      </c>
+      <c r="C113">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>565</v>
+      </c>
+      <c r="C114">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>566</v>
+      </c>
+      <c r="C115">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>567</v>
+      </c>
+      <c r="C116">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>569</v>
+      </c>
+      <c r="C117">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>571</v>
+      </c>
+      <c r="C118">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>